<commit_message>
version2 final - button shortcut was added. some error is fixed
</commit_message>
<xml_diff>
--- a/jpr_version2/configurationFile.xlsx
+++ b/jpr_version2/configurationFile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>박스</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>2개</t>
+  </si>
+  <si>
+    <t>2장</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
       <c r="D6" t="s"/>
       <c r="E6" t="s"/>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -543,11 +546,9 @@
       <c r="D7" t="s"/>
       <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G7" t="s"/>
     </row>
     <row r="8">
       <c r="A8" t="s"/>
@@ -556,7 +557,7 @@
       <c r="D8" t="s"/>
       <c r="E8" t="s"/>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s"/>
     </row>
@@ -567,7 +568,7 @@
       <c r="D9" t="s"/>
       <c r="E9" t="s"/>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s"/>
     </row>
@@ -578,7 +579,7 @@
       <c r="D10" t="s"/>
       <c r="E10" t="s"/>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s"/>
     </row>

</xml_diff>